<commit_message>
code cleanup and adding feature
</commit_message>
<xml_diff>
--- a/deliverables/Components.xlsx
+++ b/deliverables/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorecampa/eclipseProject/ProjectTIW-2021/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08B0DCB-CD09-064C-AA43-B975AB205766}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DCD90F-DD99-5247-8AD3-4C9869EB00D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5480" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{216E32EB-FD74-C341-9824-6E30DEEC878A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Beans</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>findAllPlaylistById(userId): ArrayList&lt;Playlist&gt;</t>
+  </si>
+  <si>
+    <t>AddSongToPlaylist - pOST</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="E2:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,13 +784,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="5:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:12" ht="51" x14ac:dyDescent="0.2">
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="5:12" ht="17" x14ac:dyDescent="0.2">

</xml_diff>